<commit_message>
Update Leave Card 3/14/2023 4:44 PM
</commit_message>
<xml_diff>
--- a/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
+++ b/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDB3CAD-A7A2-4A64-B5AF-3F0BEA5B6A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BC446A-13D2-4C78-BFA9-4CAA9D0E1517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -560,15 +560,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -581,11 +572,20 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3201,7 +3201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3233,7 +3233,7 @@
   <dimension ref="A2:K134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A40" activePane="bottomLeft"/>
+      <pane ySplit="3576" topLeftCell="A47" activePane="bottomLeft"/>
       <selection activeCell="F2" sqref="F2:G2"/>
       <selection pane="bottomLeft" activeCell="N48" sqref="N47:N48"/>
     </sheetView>
@@ -3263,14 +3263,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -3281,14 +3281,14 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -3299,14 +3299,14 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -3332,18 +3332,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -5661,19 +5661,19 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{DD18FAC7-4E18-48DA-ADBE-7E86BF83C85A}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
@@ -5690,8 +5690,8 @@
     <oddFooter>&amp;L
 PREPARED BY: ___________________
 DATE: &amp;D, &amp;T&amp;C
-CERTIFIED CORRECT BY: &amp;UALMA A. MALABANAN&amp;U
-                                   HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
+CERTIFIED CORRECT BY: &amp;UNANETTE B. SUSA&amp;U
+                                             OIC - HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -5740,14 +5740,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -5761,14 +5761,14 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -5779,17 +5779,17 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50" t="str">
+      <c r="F4" s="54" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -5815,18 +5815,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Leave Card 3/23/2023 4:38 PM
</commit_message>
<xml_diff>
--- a/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
+++ b/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-44REB32\Users\ASUS\Desktop\LEAVECARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BC446A-13D2-4C78-BFA9-4CAA9D0E1517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -28,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>PERIOD</t>
   </si>
@@ -180,11 +179,53 @@
   <si>
     <t>2022</t>
   </si>
+  <si>
+    <t>SL(2-0-0)</t>
+  </si>
+  <si>
+    <t>1/18,19/2018</t>
+  </si>
+  <si>
+    <t>VL(2-0-0)</t>
+  </si>
+  <si>
+    <t>3/8,9/2018</t>
+  </si>
+  <si>
+    <t>SL(1-0-0)</t>
+  </si>
+  <si>
+    <t>8/20,21/2018</t>
+  </si>
+  <si>
+    <t>VL(1-0-0)</t>
+  </si>
+  <si>
+    <t>10/23,24/2018</t>
+  </si>
+  <si>
+    <t>SP(1-0-0)</t>
+  </si>
+  <si>
+    <t>11/26,27,2018</t>
+  </si>
+  <si>
+    <t>SP(2-0-0)</t>
+  </si>
+  <si>
+    <t>12/13,14/2018</t>
+  </si>
+  <si>
+    <t>VL(3-0-0)</t>
+  </si>
+  <si>
+    <t>12/26-28/2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -415,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -560,6 +601,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -572,26 +622,23 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,7 +659,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -687,7 +733,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -755,7 +800,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -997,7 +1041,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1239,7 +1282,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1287,7 +1329,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1330,7 +1372,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1394,7 +1436,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1454,7 +1496,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1520,7 +1562,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1583,7 +1625,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1681,7 +1723,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1740,7 +1782,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1805,7 +1847,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1848,7 +1890,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,7 +1965,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2109,7 +2151,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2175,7 +2217,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2233,7 +2275,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2299,7 +2341,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2355,7 +2397,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2472,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2473,7 +2515,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2539,7 +2581,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2595,7 +2637,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2693,7 +2735,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2756,7 +2798,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2822,25 +2864,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14CC22A9-102C-45E7-BAAB-C47A27FF23A4}" name="Table15" displayName="Table15" ref="A8:K134" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A8:K134" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0C9C29E7-086E-410D-9F7F-922B65AFF7C2}" name="PERIOD" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{C0D9107B-681C-447D-9D55-1210AB62C03D}" name="PARTICULARS" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{667972B6-BE1A-43AA-953B-CB4BA1B4AE6C}" name="EARNED" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{19CA5BD7-9FF5-4CD9-B4FF-014C1678384C}" name="Absence Undertime W/ Pay" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{A9DCEC0C-0EF9-4003-85B9-B3D89C57A3EC}" name="BALANCE" dataDxfId="31">
+    <tableColumn id="1" name="PERIOD" dataDxfId="35"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="34"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="33"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="32"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="31">
       <calculatedColumnFormula>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5C8D5936-8E2A-4E52-B1B0-2666C7C86A1A}" name="Absence Undertime W/O Pay" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{28B9B9BB-F1E8-4DCF-BB6F-8D06E99BA592}" name="EARNED " dataDxfId="29">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="30"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="29">
       <calculatedColumnFormula>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{957A3318-847F-4D09-83EC-4B5896F95A97}" name="Absence Undertime  W/ Pay" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{2134A134-3E34-467C-8095-C0F6C3A6ECC2}" name="BALANCE " dataDxfId="27">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="28"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="27">
       <calculatedColumnFormula>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{54A293EB-A073-4AF9-946D-75C98B9D1944}" name="Absence Undertime  W/O Pay" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{CAFD807E-350A-4811-8B8F-DCB0B217D028}" name="REMARKS" dataDxfId="25"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="26"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2852,25 +2894,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D52DCCA-84C7-4E23-9F01-BAD20F9E44D8}" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K131" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{29298656-164E-44DD-A190-558D78410746}" name="PERIOD" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{653A013C-2253-41B2-B51E-E0CEE6FCA4B9}" name="PARTICULARS" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{23618FA7-8FE1-47F3-A791-7E4F2612427B}" name="EARNED" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{BA6D2C36-5CF4-40D7-AFDD-218AEBB26721}" name="Absence Undertime W/ Pay" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{44B79BA7-06A4-4888-BFE5-96396FB13C9E}" name="BALANCE" dataDxfId="16">
+    <tableColumn id="1" name="PERIOD" dataDxfId="20"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="19"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="18"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="17"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1A20B288-1D72-4858-B3C2-871EB9CF011E}" name="Absence Undertime W/O Pay" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{16E84B2D-53AC-4AEA-B1BC-1BC1E2E9B51B}" name="EARNED " dataDxfId="14">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="15"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A10DEDBF-F571-4518-A832-0B75654FC984}" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{9E225A68-4AC2-420E-B4D1-1378612CB5CD}" name="BALANCE " dataDxfId="12">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="12">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{715FA023-3759-440B-8D8E-42D3E30EC36F}" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{7E55BDC4-4FFC-4009-94E5-7F3F3565D56A}" name="REMARKS" dataDxfId="10"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2882,13 +2924,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB44E398-F318-4683-B466-030B39F69924}" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="D2:G3" xr:uid="{CB44E398-F318-4683-B466-030B39F69924}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="D2:G3"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1CAFD6A5-0771-4D4F-B29C-8C8A4BD59DAD}" name="DAYS"/>
-    <tableColumn id="2" xr3:uid="{D6E424DD-7C72-4461-BBE2-CD59B37123B3}" name="HOURS"/>
-    <tableColumn id="3" xr3:uid="{20858E5D-6D7D-4382-8DBC-1FD4091C418E}" name="MINUTES"/>
-    <tableColumn id="4" xr3:uid="{7FA7784E-0318-4F9C-9B40-57F4F3F3FD45}" name="EQUIVALENT HOURS" dataDxfId="5">
+    <tableColumn id="1" name="DAYS"/>
+    <tableColumn id="2" name="HOURS"/>
+    <tableColumn id="3" name="MINUTES"/>
+    <tableColumn id="4" name="EQUIVALENT HOURS" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2897,14 +2939,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CB4120CB-17DA-4A84-90C5-840D28205819}" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="J2:L3" xr:uid="{CB4120CB-17DA-4A84-90C5-840D28205819}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="J2:L3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6D76F81F-2FB2-4658-9985-FB0CE23F1771}" name="DATE STARTED" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{40B8C089-638A-4D13-9FCC-740888AE7704}" name="LEAVE EARN" dataDxfId="1">
+    <tableColumn id="1" name="DATE STARTED" dataDxfId="2"/>
+    <tableColumn id="2" name="LEAVE EARN" dataDxfId="1">
       <calculatedColumnFormula>J4-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C3A40ACA-C07A-4798-82C2-714BDF47B4DB}" name="LEAVE EARNED" dataDxfId="0">
+    <tableColumn id="3" name="LEAVE EARNED" dataDxfId="0">
       <calculatedColumnFormula>IF($J$4=1,1.25,IF(ISBLANK($J$3),"---",1.25-VLOOKUP($K$3,$I$8:$K$37,2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3208,7 +3250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D098C40-D36A-4A12-B6E1-6D049DE49862}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3218,7 +3260,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3226,34 +3268,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB84D5D2-2EE3-48FB-9BB0-C3046D30F8C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A47" activePane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3690" topLeftCell="A47" activePane="bottomLeft"/>
       <selection activeCell="F2" sqref="F2:G2"/>
       <selection pane="bottomLeft" activeCell="N48" sqref="N47:N48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -3263,16 +3305,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3281,16 +3323,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="57"/>
+      <c r="K3" s="58"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3299,16 +3341,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3316,7 +3358,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3329,24 +3371,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3405,7 +3447,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>42</v>
       </c>
@@ -3427,7 +3469,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3447,7 +3489,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3467,7 +3509,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3487,7 +3529,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3507,7 +3549,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3527,7 +3569,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -3547,7 +3589,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3567,7 +3609,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3587,7 +3629,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3607,7 +3649,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3627,7 +3669,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3647,7 +3689,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3667,7 +3709,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>43</v>
       </c>
@@ -3685,7 +3727,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3705,7 +3747,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3725,7 +3767,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3745,7 +3787,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3765,7 +3807,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3785,7 +3827,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3805,7 +3847,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -3825,7 +3867,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -3845,7 +3887,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -3865,7 +3907,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -3885,7 +3927,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -3905,7 +3947,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -3925,7 +3967,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
         <v>44</v>
       </c>
@@ -3943,7 +3985,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -3963,7 +4005,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -3983,7 +4025,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -4003,7 +4045,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -4023,7 +4065,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -4043,7 +4085,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -4063,7 +4105,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -4083,7 +4125,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -4103,7 +4145,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -4123,7 +4165,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -4143,7 +4185,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -4163,7 +4205,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -4183,7 +4225,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
         <v>45</v>
       </c>
@@ -4201,7 +4243,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -4221,7 +4263,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -4241,7 +4283,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -4261,7 +4303,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -4281,7 +4323,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -4301,7 +4343,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -4321,7 +4363,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -4341,7 +4383,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -4361,7 +4403,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -4381,7 +4423,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -4401,7 +4443,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -4421,7 +4463,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -4441,7 +4483,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
         <v>46</v>
       </c>
@@ -4459,7 +4501,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -4479,7 +4521,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -4499,7 +4541,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -4519,7 +4561,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
         <v>44652</v>
       </c>
@@ -4539,7 +4581,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40">
         <v>44682</v>
       </c>
@@ -4559,7 +4601,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
         <v>44713</v>
       </c>
@@ -4579,7 +4621,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
         <v>44743</v>
       </c>
@@ -4599,7 +4641,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>44774</v>
       </c>
@@ -4619,7 +4661,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40">
         <v>44805</v>
       </c>
@@ -4639,7 +4681,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
         <v>44835</v>
       </c>
@@ -4659,7 +4701,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40">
         <v>44866</v>
       </c>
@@ -4679,7 +4721,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
         <v>44896</v>
       </c>
@@ -4699,7 +4741,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4715,7 +4757,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4731,7 +4773,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4747,7 +4789,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4763,7 +4805,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4779,7 +4821,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4795,7 +4837,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4811,7 +4853,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4827,7 +4869,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4843,7 +4885,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4859,7 +4901,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4875,7 +4917,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4891,7 +4933,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4907,7 +4949,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4923,7 +4965,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4939,7 +4981,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4955,7 +4997,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4971,7 +5013,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4987,7 +5029,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -5003,7 +5045,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -5019,7 +5061,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -5035,7 +5077,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -5051,7 +5093,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -5067,7 +5109,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -5083,7 +5125,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -5099,7 +5141,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -5115,7 +5157,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -5131,7 +5173,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -5147,7 +5189,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -5163,7 +5205,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -5179,7 +5221,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -5195,7 +5237,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -5211,7 +5253,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -5227,7 +5269,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -5243,7 +5285,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -5259,7 +5301,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -5275,7 +5317,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -5291,7 +5333,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5307,7 +5349,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5323,7 +5365,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5339,7 +5381,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5355,7 +5397,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5371,7 +5413,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5387,7 +5429,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5403,7 +5445,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5419,7 +5461,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5435,7 +5477,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5451,7 +5493,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5467,7 +5509,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5483,7 +5525,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5499,7 +5541,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5515,7 +5557,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5531,7 +5573,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5547,7 +5589,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5563,7 +5605,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5579,7 +5621,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5595,7 +5637,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5611,7 +5653,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5627,7 +5669,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -5643,7 +5685,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="41"/>
       <c r="B134" s="15"/>
       <c r="C134" s="42"/>
@@ -5661,23 +5703,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{DD18FAC7-4E18-48DA-ADBE-7E86BF83C85A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{FBD164C5-E463-4929-8BE7-9C555DECFD39}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5700,34 +5742,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FF8E2B-FA0C-43AD-94F6-3305AF75672F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K130"/>
+  <dimension ref="A2:K131"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3570" topLeftCell="A13" activePane="bottomLeft"/>
       <selection activeCell="B2" sqref="B2:C2"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -5740,16 +5782,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -5761,16 +5803,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="57"/>
+      <c r="K3" s="58"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -5779,19 +5821,19 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54" t="str">
+      <c r="F4" s="50" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -5799,7 +5841,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -5812,24 +5854,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -5864,7 +5906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -5873,7 +5915,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>0</v>
+        <v>53.582999999999998</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -5883,13 +5925,15 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>0</v>
+        <v>85.167000000000002</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
+        <v>42</v>
+      </c>
       <c r="B10" s="20"/>
       <c r="C10" s="13"/>
       <c r="D10" s="39"/>
@@ -5908,9 +5952,13 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="20"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>43101</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C11" s="13"/>
       <c r="D11" s="39"/>
       <c r="E11" s="9"/>
@@ -5919,16 +5967,26 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H11" s="39"/>
+      <c r="H11" s="39">
+        <v>2</v>
+      </c>
       <c r="I11" s="9"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="20"/>
+      <c r="K11" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
+        <v>43160</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="39"/>
+      <c r="D12" s="39">
+        <v>2</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="20"/>
       <c r="G12" s="13" t="str">
@@ -5938,11 +5996,17 @@
       <c r="H12" s="39"/>
       <c r="I12" s="9"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="20"/>
+      <c r="K12" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="40">
+        <v>43191</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="C13" s="13"/>
       <c r="D13" s="39"/>
       <c r="E13" s="9"/>
@@ -5951,14 +6015,22 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H13" s="39"/>
+      <c r="H13" s="39">
+        <v>1</v>
+      </c>
       <c r="I13" s="9"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
-      <c r="B14" s="20"/>
+      <c r="K13" s="61">
+        <v>43203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="40">
+        <v>43252</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="C14" s="13"/>
       <c r="D14" s="39"/>
       <c r="E14" s="9"/>
@@ -5967,14 +6039,22 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H14" s="39"/>
+      <c r="H14" s="39">
+        <v>1</v>
+      </c>
       <c r="I14" s="9"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="20"/>
+      <c r="K14" s="61">
+        <v>43265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="40">
+        <v>43313</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="39"/>
       <c r="E15" s="9"/>
@@ -5983,16 +6063,26 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H15" s="39"/>
+      <c r="H15" s="39">
+        <v>2</v>
+      </c>
       <c r="I15" s="9"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
-      <c r="B16" s="15"/>
+      <c r="K15" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="41">
+        <v>43344</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
+      <c r="D16" s="43">
+        <v>1</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="15"/>
       <c r="G16" s="42" t="str">
@@ -6002,11 +6092,17 @@
       <c r="H16" s="43"/>
       <c r="I16" s="9"/>
       <c r="J16" s="12"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="20"/>
+      <c r="K16" s="62">
+        <v>43363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>43374</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="C17" s="13"/>
       <c r="D17" s="39"/>
       <c r="E17" s="9"/>
@@ -6015,16 +6111,24 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H17" s="39"/>
+      <c r="H17" s="39">
+        <v>1</v>
+      </c>
       <c r="I17" s="9"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K17" s="61">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="39"/>
+      <c r="D18" s="39">
+        <v>2</v>
+      </c>
       <c r="E18" s="9"/>
       <c r="F18" s="20"/>
       <c r="G18" s="13" t="str">
@@ -6034,11 +6138,17 @@
       <c r="H18" s="39"/>
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="20"/>
+      <c r="K18" s="61" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
+        <v>43405</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="13"/>
       <c r="D19" s="39"/>
       <c r="E19" s="9"/>
@@ -6050,11 +6160,15 @@
       <c r="H19" s="39"/>
       <c r="I19" s="9"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="20"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="61">
+        <v>43423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
-      <c r="B20" s="20"/>
+      <c r="B20" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C20" s="13"/>
       <c r="D20" s="39"/>
       <c r="E20" s="9"/>
@@ -6063,14 +6177,22 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H20" s="39"/>
+      <c r="H20" s="39">
+        <v>2</v>
+      </c>
       <c r="I20" s="9"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="20"/>
+      <c r="K20" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="40">
+        <v>43435</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C21" s="13"/>
       <c r="D21" s="39"/>
       <c r="E21" s="9"/>
@@ -6082,13 +6204,19 @@
       <c r="H21" s="39"/>
       <c r="I21" s="9"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K21" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
-      <c r="B22" s="20"/>
+      <c r="B22" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="39"/>
+      <c r="D22" s="39">
+        <v>3</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="20"/>
       <c r="G22" s="13" t="str">
@@ -6098,9 +6226,11 @@
       <c r="H22" s="39"/>
       <c r="I22" s="9"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="20"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K22" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="20"/>
       <c r="C23" s="13"/>
@@ -6116,7 +6246,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="20"/>
       <c r="C24" s="13"/>
@@ -6132,7 +6262,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="20"/>
       <c r="C25" s="13"/>
@@ -6148,7 +6278,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="20"/>
       <c r="C26" s="13"/>
@@ -6164,7 +6294,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
@@ -6180,7 +6310,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="20"/>
       <c r="C28" s="13"/>
@@ -6196,7 +6326,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
       <c r="B29" s="20"/>
       <c r="C29" s="13"/>
@@ -6212,7 +6342,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -6228,7 +6358,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="20"/>
       <c r="C31" s="13"/>
@@ -6244,7 +6374,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
@@ -6260,7 +6390,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -6276,7 +6406,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -6292,7 +6422,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -6308,7 +6438,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -6324,7 +6454,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -6340,7 +6470,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -6356,7 +6486,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -6372,7 +6502,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -6388,7 +6518,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -6404,7 +6534,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -6420,7 +6550,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -6436,7 +6566,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -6452,7 +6582,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -6468,7 +6598,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -6484,7 +6614,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -6500,7 +6630,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -6516,7 +6646,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -6532,7 +6662,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -6548,7 +6678,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -6564,7 +6694,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -6580,7 +6710,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -6596,7 +6726,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -6612,7 +6742,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -6628,7 +6758,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -6644,7 +6774,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -6660,7 +6790,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -6676,7 +6806,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -6692,7 +6822,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -6708,7 +6838,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -6724,7 +6854,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -6740,7 +6870,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -6756,7 +6886,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -6772,7 +6902,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -6788,7 +6918,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -6804,7 +6934,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -6820,7 +6950,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -6836,7 +6966,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -6852,7 +6982,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -6868,7 +6998,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -6884,7 +7014,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -6900,7 +7030,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -6916,7 +7046,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -6932,7 +7062,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -6948,7 +7078,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -6964,7 +7094,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -6980,7 +7110,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -6996,7 +7126,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -7012,7 +7142,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -7028,7 +7158,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -7044,7 +7174,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -7060,7 +7190,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -7076,7 +7206,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -7092,7 +7222,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -7108,7 +7238,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -7124,7 +7254,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -7140,7 +7270,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -7156,7 +7286,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -7172,7 +7302,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -7188,7 +7318,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -7204,7 +7334,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -7220,7 +7350,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -7236,7 +7366,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -7252,7 +7382,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -7268,7 +7398,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -7284,7 +7414,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -7300,7 +7430,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -7316,7 +7446,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -7332,7 +7462,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -7348,7 +7478,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -7364,7 +7494,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -7380,7 +7510,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -7396,7 +7526,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -7412,7 +7542,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -7428,7 +7558,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -7444,7 +7574,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -7460,7 +7590,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -7476,7 +7606,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -7492,7 +7622,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -7508,7 +7638,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -7524,7 +7654,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -7540,7 +7670,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -7556,7 +7686,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -7572,7 +7702,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -7588,7 +7718,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -7604,7 +7734,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -7620,7 +7750,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -7636,7 +7766,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -7652,7 +7782,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -7668,7 +7798,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -7684,7 +7814,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -7700,7 +7830,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -7716,7 +7846,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -7732,7 +7862,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -7748,7 +7878,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -7764,7 +7894,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -7780,7 +7910,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -7796,7 +7926,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -7812,21 +7942,37 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A130" s="41"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="42"/>
-      <c r="D130" s="43"/>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130" s="40"/>
+      <c r="B130" s="20"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="39"/>
       <c r="E130" s="9"/>
-      <c r="F130" s="15"/>
-      <c r="G130" s="42" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H130" s="43"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H130" s="39"/>
       <c r="I130" s="9"/>
-      <c r="J130" s="12"/>
-      <c r="K130" s="15"/>
+      <c r="J130" s="11"/>
+      <c r="K130" s="20"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131" s="41"/>
+      <c r="B131" s="15"/>
+      <c r="C131" s="42"/>
+      <c r="D131" s="43"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="42" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H131" s="43"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="12"/>
+      <c r="K131" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7843,10 +7989,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{3C67B38A-DE91-4BA1-85D0-F5C61D6395E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{C9F25C0C-606E-415B-87B4-B098DE141EB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7869,29 +8015,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB8F789-193C-43F9-8D48-B0DEE5C76ADA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="59" t="s">
         <v>33</v>
       </c>
@@ -7904,7 +8050,7 @@
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -7933,9 +8079,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>61.582999999999998</v>
+      </c>
+      <c r="B3" s="11">
+        <v>94.167000000000002</v>
+      </c>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -7953,17 +8103,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -7984,7 +8134,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -8011,7 +8161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -8037,7 +8187,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -8063,7 +8213,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -8089,7 +8239,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -8115,7 +8265,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -8141,7 +8291,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -8167,7 +8317,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -8193,7 +8343,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -8213,7 +8363,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -8233,7 +8383,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -8253,7 +8403,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -8274,7 +8424,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -8295,7 +8445,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -8316,7 +8466,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -8337,7 +8487,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -8358,7 +8508,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -8379,7 +8529,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -8400,7 +8550,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -8421,7 +8571,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -8442,7 +8592,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -8463,7 +8613,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -8484,7 +8634,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -8505,7 +8655,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -8526,7 +8676,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -8547,7 +8697,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -8568,7 +8718,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -8589,7 +8739,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -8610,7 +8760,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -8631,7 +8781,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -8652,7 +8802,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -8673,7 +8823,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -8682,7 +8832,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -8691,7 +8841,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -8700,7 +8850,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -8709,7 +8859,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -8718,7 +8868,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -8727,7 +8877,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -8736,7 +8886,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -8745,7 +8895,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -8754,7 +8904,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -8763,7 +8913,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -8772,7 +8922,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -8781,7 +8931,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -8790,7 +8940,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -8799,7 +8949,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -8808,7 +8958,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -8817,7 +8967,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -8826,7 +8976,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -8835,7 +8985,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -8844,7 +8994,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -8853,7 +9003,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -8862,7 +9012,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -8871,7 +9021,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -8880,7 +9030,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -8889,7 +9039,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -8898,7 +9048,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -8907,7 +9057,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -8916,7 +9066,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -8925,7 +9075,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -8934,7 +9084,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
CARLA UPDATE LEAVE CARD 4/4/2023 11:50 PM
</commit_message>
<xml_diff>
--- a/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
+++ b/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-44REB32\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301B575D-1616-48DE-B736-C3812CF2AB5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -27,7 +28,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>PERIOD</t>
   </si>
@@ -180,57 +181,19 @@
     <t>2022</t>
   </si>
   <si>
-    <t>SL(2-0-0)</t>
-  </si>
-  <si>
-    <t>1/18,19/2018</t>
-  </si>
-  <si>
-    <t>VL(2-0-0)</t>
-  </si>
-  <si>
-    <t>3/8,9/2018</t>
-  </si>
-  <si>
-    <t>SL(1-0-0)</t>
-  </si>
-  <si>
-    <t>8/20,21/2018</t>
-  </si>
-  <si>
-    <t>VL(1-0-0)</t>
-  </si>
-  <si>
-    <t>10/23,24/2018</t>
-  </si>
-  <si>
-    <t>SP(1-0-0)</t>
-  </si>
-  <si>
-    <t>11/26,27,2018</t>
-  </si>
-  <si>
-    <t>SP(2-0-0)</t>
-  </si>
-  <si>
-    <t>12/13,14/2018</t>
-  </si>
-  <si>
-    <t>VL(3-0-0)</t>
-  </si>
-  <si>
-    <t>12/26-28/2018</t>
+    <t>TOTAL LEAVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="166" formatCode="###\-###\-###"/>
     <numFmt numFmtId="167" formatCode="&quot;CM&quot;\-#######"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -456,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,17 +561,14 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -622,11 +582,20 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -634,10 +603,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1329,7 +1298,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,7 +1341,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1405,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1496,7 +1465,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,7 +1531,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1625,7 +1594,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1723,7 +1692,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1782,7 +1751,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1847,7 +1816,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1890,7 +1859,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1965,7 +1934,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2151,7 +2120,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2217,7 +2186,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2275,7 +2244,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2341,7 +2310,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2397,7 +2366,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2472,7 +2441,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2515,7 +2484,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2581,7 +2550,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2637,7 +2606,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2735,7 +2704,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2798,7 +2767,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2864,25 +2833,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A8:K134" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A8:K134" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="35"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="34"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="33"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="32"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="31">
       <calculatedColumnFormula>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="30"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="29">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="29">
       <calculatedColumnFormula>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="28"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="27">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="27">
       <calculatedColumnFormula>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="26"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2894,25 +2863,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K131" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K131" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="20"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="19"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="18"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="17"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="15"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="12">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="12">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2924,13 +2893,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="D2:G3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="D2:G3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="DAYS"/>
-    <tableColumn id="2" name="HOURS"/>
-    <tableColumn id="3" name="MINUTES"/>
-    <tableColumn id="4" name="EQUIVALENT HOURS" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="DAYS"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="HOURS"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="MINUTES"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="EQUIVALENT HOURS" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2939,14 +2908,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="J2:L3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="J2:L3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="DATE STARTED" dataDxfId="2"/>
-    <tableColumn id="2" name="LEAVE EARN" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE STARTED" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="LEAVE EARN" dataDxfId="1">
       <calculatedColumnFormula>J4-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="LEAVE EARNED" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="LEAVE EARNED" dataDxfId="0">
       <calculatedColumnFormula>IF($J$4=1,1.25,IF(ISBLANK($J$3),"---",1.25-VLOOKUP($K$3,$I$8:$K$37,2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3250,7 +3219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3260,7 +3229,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3268,63 +3237,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K134"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A47" activePane="bottomLeft"/>
+      <pane ySplit="3696" activePane="bottomLeft"/>
       <selection activeCell="F2" sqref="F2:G2"/>
-      <selection pane="bottomLeft" activeCell="N48" sqref="N47:N48"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
@@ -3332,25 +3301,25 @@
       <c r="J3" s="57"/>
       <c r="K3" s="58"/>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="56"/>
+      <c r="K4" s="59"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3358,7 +3327,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3371,24 +3340,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3423,7 +3392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3447,7 +3416,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>42</v>
       </c>
@@ -3469,7 +3438,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3489,7 +3458,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3509,7 +3478,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3529,7 +3498,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3549,7 +3518,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3569,7 +3538,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -3589,7 +3558,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3609,7 +3578,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3629,7 +3598,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3649,7 +3618,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3669,7 +3638,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3689,7 +3658,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3709,7 +3678,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>43</v>
       </c>
@@ -3727,7 +3696,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3747,7 +3716,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3767,7 +3736,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3787,7 +3756,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3807,7 +3776,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3827,7 +3796,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3847,7 +3816,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -3867,7 +3836,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -3887,7 +3856,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -3907,7 +3876,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -3927,7 +3896,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -3947,7 +3916,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -3967,7 +3936,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>44</v>
       </c>
@@ -3985,7 +3954,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -4005,7 +3974,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -4025,7 +3994,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -4045,7 +4014,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -4065,7 +4034,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -4085,7 +4054,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -4105,7 +4074,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -4125,7 +4094,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -4145,7 +4114,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -4165,7 +4134,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -4185,7 +4154,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -4205,7 +4174,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -4225,7 +4194,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="48" t="s">
         <v>45</v>
       </c>
@@ -4243,7 +4212,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -4263,7 +4232,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -4283,7 +4252,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -4303,7 +4272,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -4323,7 +4292,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -4343,7 +4312,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -4363,7 +4332,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -4383,7 +4352,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -4403,7 +4372,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -4423,7 +4392,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -4443,7 +4412,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -4463,7 +4432,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -4483,7 +4452,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="48" t="s">
         <v>46</v>
       </c>
@@ -4501,7 +4470,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -4521,7 +4490,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -4541,7 +4510,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -4561,7 +4530,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40">
         <v>44652</v>
       </c>
@@ -4581,7 +4550,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40">
         <v>44682</v>
       </c>
@@ -4601,7 +4570,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40">
         <v>44713</v>
       </c>
@@ -4621,7 +4590,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">
         <v>44743</v>
       </c>
@@ -4641,7 +4610,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40">
         <v>44774</v>
       </c>
@@ -4661,7 +4630,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
         <v>44805</v>
       </c>
@@ -4681,7 +4650,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40">
         <v>44835</v>
       </c>
@@ -4701,7 +4670,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40">
         <v>44866</v>
       </c>
@@ -4721,7 +4690,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
         <v>44896</v>
       </c>
@@ -4741,7 +4710,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4757,7 +4726,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4773,7 +4742,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4789,7 +4758,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4805,7 +4774,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4821,7 +4790,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4837,7 +4806,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4853,7 +4822,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4869,7 +4838,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4885,7 +4854,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4901,7 +4870,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4917,7 +4886,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4933,7 +4902,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4949,7 +4918,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4965,7 +4934,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4981,7 +4950,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4997,7 +4966,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -5013,7 +4982,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -5029,7 +4998,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -5045,7 +5014,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -5061,7 +5030,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -5077,7 +5046,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -5093,7 +5062,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -5109,7 +5078,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -5125,7 +5094,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -5141,7 +5110,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -5157,7 +5126,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -5173,7 +5142,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -5189,7 +5158,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -5205,7 +5174,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -5221,7 +5190,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -5237,7 +5206,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -5253,7 +5222,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -5269,7 +5238,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -5285,7 +5254,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -5301,7 +5270,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -5317,7 +5286,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -5333,7 +5302,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5349,7 +5318,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5365,7 +5334,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5381,7 +5350,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5397,7 +5366,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5413,7 +5382,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5429,7 +5398,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5445,7 +5414,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5461,7 +5430,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5477,7 +5446,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5493,7 +5462,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5509,7 +5478,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5525,7 +5494,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5541,7 +5510,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5557,7 +5526,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5573,7 +5542,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5589,7 +5558,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5605,7 +5574,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5621,7 +5590,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5637,7 +5606,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5653,7 +5622,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5669,7 +5638,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -5685,7 +5654,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="41"/>
       <c r="B134" s="15"/>
       <c r="C134" s="42"/>
@@ -5703,23 +5672,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5742,69 +5711,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3570" topLeftCell="A13" activePane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2:C2"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3576" topLeftCell="A5"/>
+      <selection activeCell="J2" sqref="J2:K2"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="51" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B2:C2),"---------",'2018 LEAVE CREDITS'!B2:C2)</f>
         <v>---------</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="51" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B3:C3),"",'2018 LEAVE CREDITS'!B3:C3)</f>
         <v/>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
@@ -5812,28 +5781,28 @@
       <c r="J3" s="57"/>
       <c r="K3" s="58"/>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50" t="str">
+      <c r="F4" s="56" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="56"/>
+      <c r="K4" s="59"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -5841,7 +5810,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -5854,24 +5823,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -5906,7 +5875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -5915,7 +5884,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>53.582999999999998</v>
+        <v>0</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -5925,12 +5894,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>85.167000000000002</v>
+        <v>0</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>42</v>
       </c>
@@ -5952,13 +5921,9 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
-        <v>43101</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>47</v>
-      </c>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="40"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="13"/>
       <c r="D11" s="39"/>
       <c r="E11" s="9"/>
@@ -5967,26 +5932,16 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H11" s="39">
-        <v>2</v>
-      </c>
+      <c r="H11" s="39"/>
       <c r="I11" s="9"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
-        <v>43160</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="39">
-        <v>2</v>
-      </c>
+      <c r="D12" s="39"/>
       <c r="E12" s="9"/>
       <c r="F12" s="20"/>
       <c r="G12" s="13" t="str">
@@ -5996,17 +5951,11 @@
       <c r="H12" s="39"/>
       <c r="I12" s="9"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="40">
-        <v>43191</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="40"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="13"/>
       <c r="D13" s="39"/>
       <c r="E13" s="9"/>
@@ -6015,22 +5964,14 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H13" s="39">
-        <v>1</v>
-      </c>
+      <c r="H13" s="39"/>
       <c r="I13" s="9"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="61">
-        <v>43203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="40">
-        <v>43252</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="K13" s="49"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="13"/>
       <c r="D14" s="39"/>
       <c r="E14" s="9"/>
@@ -6039,22 +5980,14 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H14" s="39">
-        <v>1</v>
-      </c>
+      <c r="H14" s="39"/>
       <c r="I14" s="9"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="61">
-        <v>43265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="40">
-        <v>43313</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="K14" s="49"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="13"/>
       <c r="D15" s="39"/>
       <c r="E15" s="9"/>
@@ -6063,26 +5996,16 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H15" s="39">
-        <v>2</v>
-      </c>
+      <c r="H15" s="39"/>
       <c r="I15" s="9"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="41">
-        <v>43344</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>53</v>
-      </c>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="41"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="42"/>
-      <c r="D16" s="43">
-        <v>1</v>
-      </c>
+      <c r="D16" s="43"/>
       <c r="E16" s="9"/>
       <c r="F16" s="15"/>
       <c r="G16" s="42" t="str">
@@ -6092,17 +6015,11 @@
       <c r="H16" s="43"/>
       <c r="I16" s="9"/>
       <c r="J16" s="12"/>
-      <c r="K16" s="62">
-        <v>43363</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="40">
-        <v>43374</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="K16" s="50"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="40"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="13"/>
       <c r="D17" s="39"/>
       <c r="E17" s="9"/>
@@ -6111,24 +6028,16 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H17" s="39">
-        <v>1</v>
-      </c>
+      <c r="H17" s="39"/>
       <c r="I17" s="9"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="61">
-        <v>43384</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="49"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40"/>
-      <c r="B18" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="B18" s="20"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="39">
-        <v>2</v>
-      </c>
+      <c r="D18" s="39"/>
       <c r="E18" s="9"/>
       <c r="F18" s="20"/>
       <c r="G18" s="13" t="str">
@@ -6138,17 +6047,11 @@
       <c r="H18" s="39"/>
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="40">
-        <v>43405</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="K18" s="49"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="40"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="13"/>
       <c r="D19" s="39"/>
       <c r="E19" s="9"/>
@@ -6160,15 +6063,11 @@
       <c r="H19" s="39"/>
       <c r="I19" s="9"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="61">
-        <v>43423</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="49"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40"/>
-      <c r="B20" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="B20" s="20"/>
       <c r="C20" s="13"/>
       <c r="D20" s="39"/>
       <c r="E20" s="9"/>
@@ -6177,22 +6076,14 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H20" s="39">
-        <v>2</v>
-      </c>
+      <c r="H20" s="39"/>
       <c r="I20" s="9"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="40">
-        <v>43435</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>57</v>
-      </c>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="13"/>
       <c r="D21" s="39"/>
       <c r="E21" s="9"/>
@@ -6204,19 +6095,13 @@
       <c r="H21" s="39"/>
       <c r="I21" s="9"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
-      <c r="B22" s="20" t="s">
-        <v>59</v>
-      </c>
+      <c r="B22" s="20"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="39">
-        <v>3</v>
-      </c>
+      <c r="D22" s="39"/>
       <c r="E22" s="9"/>
       <c r="F22" s="20"/>
       <c r="G22" s="13" t="str">
@@ -6226,11 +6111,9 @@
       <c r="H22" s="39"/>
       <c r="I22" s="9"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
       <c r="B23" s="20"/>
       <c r="C23" s="13"/>
@@ -6246,7 +6129,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
       <c r="B24" s="20"/>
       <c r="C24" s="13"/>
@@ -6262,7 +6145,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
       <c r="B25" s="20"/>
       <c r="C25" s="13"/>
@@ -6278,7 +6161,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
       <c r="B26" s="20"/>
       <c r="C26" s="13"/>
@@ -6294,7 +6177,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
@@ -6310,7 +6193,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="20"/>
       <c r="C28" s="13"/>
@@ -6326,7 +6209,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
       <c r="B29" s="20"/>
       <c r="C29" s="13"/>
@@ -6342,7 +6225,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -6358,7 +6241,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
       <c r="B31" s="20"/>
       <c r="C31" s="13"/>
@@ -6374,7 +6257,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
@@ -6390,7 +6273,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -6406,7 +6289,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -6422,7 +6305,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -6438,7 +6321,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40"/>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -6454,7 +6337,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -6470,7 +6353,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -6486,7 +6369,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -6502,7 +6385,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -6518,7 +6401,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -6534,7 +6417,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -6550,7 +6433,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -6566,7 +6449,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -6582,7 +6465,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -6598,7 +6481,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -6614,7 +6497,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -6630,7 +6513,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -6646,7 +6529,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -6662,7 +6545,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -6678,7 +6561,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -6694,7 +6577,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -6710,7 +6593,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -6726,7 +6609,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -6742,7 +6625,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -6758,7 +6641,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -6774,7 +6657,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -6790,7 +6673,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -6806,7 +6689,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -6822,7 +6705,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -6838,7 +6721,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -6854,7 +6737,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -6870,7 +6753,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -6886,7 +6769,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -6902,7 +6785,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -6918,7 +6801,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -6934,7 +6817,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -6950,7 +6833,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -6966,7 +6849,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -6982,7 +6865,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -6998,7 +6881,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -7014,7 +6897,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -7030,7 +6913,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -7046,7 +6929,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -7062,7 +6945,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -7078,7 +6961,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -7094,7 +6977,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -7110,7 +6993,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -7126,7 +7009,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -7142,7 +7025,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -7158,7 +7041,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -7174,7 +7057,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -7190,7 +7073,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -7206,7 +7089,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -7222,7 +7105,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -7238,7 +7121,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -7254,7 +7137,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -7270,7 +7153,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -7286,7 +7169,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -7302,7 +7185,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -7318,7 +7201,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -7334,7 +7217,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -7350,7 +7233,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -7366,7 +7249,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -7382,7 +7265,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -7398,7 +7281,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -7414,7 +7297,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -7430,7 +7313,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -7446,7 +7329,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -7462,7 +7345,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -7478,7 +7361,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -7494,7 +7377,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -7510,7 +7393,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -7526,7 +7409,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -7542,7 +7425,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -7558,7 +7441,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -7574,7 +7457,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -7590,7 +7473,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -7606,7 +7489,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -7622,7 +7505,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -7638,7 +7521,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -7654,7 +7537,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -7670,7 +7553,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -7686,7 +7569,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -7702,7 +7585,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -7718,7 +7601,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -7734,7 +7617,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -7750,7 +7633,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -7766,7 +7649,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -7782,7 +7665,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -7798,7 +7681,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -7814,7 +7697,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -7830,7 +7713,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -7846,7 +7729,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -7862,7 +7745,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -7878,7 +7761,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -7894,7 +7777,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -7910,7 +7793,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -7926,7 +7809,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -7942,7 +7825,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -7958,7 +7841,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="41"/>
       <c r="B131" s="15"/>
       <c r="C131" s="42"/>
@@ -7989,10 +7872,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8015,42 +7898,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="59" t="s">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D1" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="J1" s="60" t="s">
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="J1" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -8079,13 +7962,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>61.582999999999998</v>
-      </c>
-      <c r="B3" s="11">
-        <v>94.167000000000002</v>
-      </c>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -8103,17 +7982,20 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="64" t="s">
+        <v>47</v>
+      </c>
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -8127,14 +8009,18 @@
         <v>30</v>
       </c>
       <c r="G6" s="44"/>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="63">
+        <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
+        <v>150</v>
+      </c>
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -8161,7 +8047,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -8187,7 +8073,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -8213,7 +8099,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -8239,7 +8125,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -8265,7 +8151,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -8291,7 +8177,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -8317,7 +8203,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -8343,7 +8229,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -8363,7 +8249,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -8383,7 +8269,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -8403,7 +8289,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -8424,7 +8310,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -8445,7 +8331,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -8466,7 +8352,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -8487,7 +8373,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -8508,7 +8394,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -8529,7 +8415,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -8550,7 +8436,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -8571,7 +8457,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -8592,7 +8478,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -8613,7 +8499,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -8634,7 +8520,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -8655,7 +8541,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -8676,7 +8562,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -8697,7 +8583,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -8718,7 +8604,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -8739,7 +8625,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -8760,7 +8646,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -8781,7 +8667,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -8802,7 +8688,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -8823,7 +8709,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -8832,7 +8718,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -8841,7 +8727,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -8850,7 +8736,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -8859,7 +8745,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -8868,7 +8754,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -8877,7 +8763,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -8886,7 +8772,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -8895,7 +8781,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -8904,7 +8790,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -8913,7 +8799,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -8922,7 +8808,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -8931,7 +8817,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -8940,7 +8826,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -8949,7 +8835,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -8958,7 +8844,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -8967,7 +8853,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -8976,7 +8862,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -8985,7 +8871,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -8994,7 +8880,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -9003,7 +8889,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -9012,7 +8898,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -9021,7 +8907,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -9030,7 +8916,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -9039,7 +8925,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -9048,7 +8934,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -9057,7 +8943,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -9066,7 +8952,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -9075,7 +8961,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -9084,7 +8970,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Update Leave Card 7/12/2023 10:47 AM
</commit_message>
<xml_diff>
--- a/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
+++ b/1-TEMPALTE LEAVE CARD-CASUAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301B575D-1616-48DE-B736-C3812CF2AB5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFFC683-BC80-469C-B45A-3598BD97E626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -567,8 +567,23 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -582,32 +597,17 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2816,7 +2816,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -3243,10 +3243,10 @@
   </sheetPr>
   <dimension ref="A2:K134"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" activePane="bottomLeft"/>
-      <selection activeCell="F2" sqref="F2:G2"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696"/>
+      <selection activeCell="F3" sqref="F3:G3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3268,56 +3268,56 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="62"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="59"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="55"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -3343,18 +3343,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -5672,19 +5672,19 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
@@ -5719,7 +5719,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3576" topLeftCell="A5"/>
-      <selection activeCell="J2" sqref="J2:K2"/>
+      <selection activeCell="F4" sqref="F4:G4"/>
       <selection pane="bottomLeft" activeCell="H11" sqref="H11:K22"/>
     </sheetView>
   </sheetViews>
@@ -5742,65 +5742,68 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="str">
+      <c r="B2" s="53" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B2:C2),"---------",'2018 LEAVE CREDITS'!B2:C2)</f>
         <v>---------</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51" t="str">
+      <c r="B3" s="53" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B3:C3),"",'2018 LEAVE CREDITS'!B3:C3)</f>
         <v/>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="F3" s="60" t="str">
+        <f>IF(ISBLANK('2018 LEAVE CREDITS'!F3:G3),"---------",'2018 LEAVE CREDITS'!F3:G3)</f>
+        <v>---------</v>
+      </c>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="62"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="56" t="str">
+      <c r="F4" s="54" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="56"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="59"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="55"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -5826,18 +5829,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -7902,7 +7905,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
@@ -7921,17 +7924,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="J1" s="62" t="s">
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="J1" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -7993,7 +7996,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="52" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="38" t="s">
@@ -8009,15 +8012,15 @@
         <v>30</v>
       </c>
       <c r="G6" s="44"/>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="63">
+      <c r="A7" s="51">
         <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
         <v>150</v>
       </c>

</xml_diff>